<commit_message>
changed MyClinData references to OhSnap references
</commit_message>
<xml_diff>
--- a/CBC.xlsx
+++ b/CBC.xlsx
@@ -340,7 +340,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:V1"/>
+  <dimension ref="A1:Q1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -354,107 +354,82 @@
       </c>
       <c r="B1" t="inlineStr">
         <is>
-          <t>Na</t>
+          <t>WBC</t>
         </is>
       </c>
       <c r="C1" t="inlineStr">
         <is>
-          <t>K</t>
+          <t>RBC</t>
         </is>
       </c>
       <c r="D1" t="inlineStr">
         <is>
-          <t>Cl</t>
+          <t>HGB</t>
         </is>
       </c>
       <c r="E1" t="inlineStr">
         <is>
-          <t>ECO2</t>
+          <t>HCT</t>
         </is>
       </c>
       <c r="F1" t="inlineStr">
         <is>
-          <t>AGAP</t>
+          <t>MCV</t>
         </is>
       </c>
       <c r="G1" t="inlineStr">
         <is>
-          <t>AHOL</t>
+          <t>MCH</t>
         </is>
       </c>
       <c r="H1" t="inlineStr">
         <is>
-          <t>TBI</t>
+          <t>MCHC</t>
         </is>
       </c>
       <c r="I1" t="inlineStr">
         <is>
-          <t>TP</t>
+          <t>PLT</t>
         </is>
       </c>
       <c r="J1" t="inlineStr">
         <is>
-          <t>GLOB</t>
+          <t>RDW-SD</t>
         </is>
       </c>
       <c r="K1" t="inlineStr">
         <is>
-          <t>ALPI</t>
+          <t>RDW-CV</t>
         </is>
       </c>
       <c r="L1" t="inlineStr">
         <is>
-          <t>TGL</t>
+          <t>MPV</t>
         </is>
       </c>
       <c r="M1" t="inlineStr">
         <is>
-          <t>CHOL</t>
+          <t>NEUT</t>
         </is>
       </c>
       <c r="N1" t="inlineStr">
         <is>
-          <t>AST</t>
+          <t>LYMPH</t>
         </is>
       </c>
       <c r="O1" t="inlineStr">
         <is>
-          <t>ALTI</t>
+          <t>MONO</t>
         </is>
       </c>
       <c r="P1" t="inlineStr">
         <is>
-          <t>ALB</t>
+          <t>EO</t>
         </is>
       </c>
       <c r="Q1" t="inlineStr">
         <is>
-          <t>A/G</t>
-        </is>
-      </c>
-      <c r="R1" t="inlineStr">
-        <is>
-          <t>GLUC</t>
-        </is>
-      </c>
-      <c r="S1" t="inlineStr">
-        <is>
-          <t>BUN</t>
-        </is>
-      </c>
-      <c r="T1" t="inlineStr">
-        <is>
-          <t>CA</t>
-        </is>
-      </c>
-      <c r="U1" t="inlineStr">
-        <is>
-          <t>CRE2</t>
-        </is>
-      </c>
-      <c r="V1" t="inlineStr">
-        <is>
-          <t>BN/CR</t>
+          <t>BASO</t>
         </is>
       </c>
     </row>

</xml_diff>